<commit_message>
Added more result files
</commit_message>
<xml_diff>
--- a/paper/documents/log3-22.xlsx
+++ b/paper/documents/log3-22.xlsx
@@ -702,10 +702,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>logCsv!$H$2:$H$28</c:f>
+              <c:f>logCsv!$H$2:$H$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="121"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -786,6 +786,282 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>370.566025719028</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>444.91628593886298</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>444.91628593886298</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>310.22553661141001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>310.22553661141001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>396.57065148310198</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>444.58975572279599</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>444.58975572279599</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>445.58589874099602</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>453.23312063998799</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>512.317409397338</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>538.94624827593304</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>366.18216772156399</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>522.02507982748398</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>538.94624827593304</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>538.94624827593304</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>376.488542110776</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>485.50044499686999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>530.45523209496002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>425.304259901607</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>390.19653270566499</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>428.07770015489001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>460.22053226189701</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>473.905886833088</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>421.00730397224902</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>306.50225148772</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>471.757528457273</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>267.20344062837199</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>517.52365965185095</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>361.65957176648402</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>576.54274471954295</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>363.45933694383501</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>577.33830246562502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1023,14 +1299,14 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>logCsv!$A$29</c:f>
+              <c:f>logCsv!$A$124</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1059,10 +1335,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>logCsv!$B$29:$I$29</c:f>
+              <c:f>logCsv!$B$124:$AJ$124</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>461.12158620230099</c:v>
                 </c:pt>
@@ -1086,6 +1362,87 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>505.98692982442702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>505.98692982442702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>505.98692982442702</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>505.98692982442702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>505.98692982442702</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>552.15685128966595</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>577.33830246562502</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>577.33830246562502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,7 +1450,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1973-4AD0-A145-9B42BA656098}"/>
+              <c16:uniqueId val="{00000000-E7C2-431E-8CD7-8C6CA2B4E7D4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1106,11 +1463,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="227246480"/>
-        <c:axId val="227249104"/>
+        <c:axId val="342101672"/>
+        <c:axId val="342097080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="227246480"/>
+        <c:axId val="342101672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1508,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227249104"/>
+        <c:crossAx val="342097080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1159,7 +1516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="227249104"/>
+        <c:axId val="342097080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1566,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227246480"/>
+        <c:crossAx val="342101672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1222,7 +1579,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2346,13 +2703,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>333373</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -2376,19 +2733,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>323849</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2703,10 +3060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:AJ124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="AJ125" sqref="AJ125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,7 +3484,7 @@
         <v>331.06998554178699</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.3951030677587601</v>
       </c>
@@ -3153,7 +3510,7 @@
         <v>316.73487005657398</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2.6970619055654099</v>
       </c>
@@ -3179,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.6970619055654099</v>
       </c>
@@ -3205,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.3951030677587601</v>
       </c>
@@ -3231,7 +3588,7 @@
         <v>444.56902891015199</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2.6970619055654099</v>
       </c>
@@ -3257,7 +3614,7 @@
         <v>505.98692982442702</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.3951030677587601</v>
       </c>
@@ -3283,7 +3640,7 @@
         <v>243.21802504560301</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2.3362303142763499</v>
       </c>
@@ -3309,7 +3666,7 @@
         <v>393.07069729012801</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.3951030677587601</v>
       </c>
@@ -3335,7 +3692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2.3951030677587601</v>
       </c>
@@ -3361,7 +3718,7 @@
         <v>444.56902891015199</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2.3951030677587601</v>
       </c>
@@ -3387,7 +3744,7 @@
         <v>444.89545621115099</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2.3951030677587601</v>
       </c>
@@ -3413,7 +3770,7 @@
         <v>433.205481975846</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2.6970619055654099</v>
       </c>
@@ -3439,33 +3796,2552 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B29">
+        <v>5.5315691214098104</v>
+      </c>
+      <c r="C29">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D29">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E29">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G29">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2.0774656753791398</v>
+      </c>
+      <c r="B30">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C30">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D30">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E30">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G30">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B31">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C31">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D31">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E31">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G31">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H31">
+        <v>370.566025719028</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B32">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C32">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D32">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E32">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G32">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B33">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C33">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D33">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E33">
+        <v>9.0783540995096806E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G33">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B34">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C34">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D34">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E34">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G34">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H34">
+        <v>444.91628593886298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B35">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C35">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D35">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E35">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G35">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H35">
+        <v>444.91628593886298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B36">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C36">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D36">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E36">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>8.7346677036404701E-4</v>
+      </c>
+      <c r="G36">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B37">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C37">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D37">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E37">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G37">
+        <v>6.9358240024477496E-3</v>
+      </c>
+      <c r="H37">
+        <v>310.22553661141001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B38">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C38">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D38">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E38">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F38" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G38">
+        <v>6.9358240024477496E-3</v>
+      </c>
+      <c r="H38">
+        <v>310.22553661141001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B39">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C39">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D39">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E39">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>8.7346677036404701E-4</v>
+      </c>
+      <c r="G39">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5.1713556656154704</v>
+      </c>
+      <c r="B40">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C40">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D40">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E40">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G40">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H40">
+        <v>396.57065148310198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B41">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C41">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D41">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E41">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G41">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H41">
+        <v>444.58975572279599</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B42">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C42">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D42">
+        <v>5.6320598019593202</v>
+      </c>
+      <c r="E42">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G42">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H42">
+        <v>444.58975572279599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5.90142417538899</v>
+      </c>
+      <c r="B43">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C43">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D43">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E43">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>8.7346677036404701E-4</v>
+      </c>
+      <c r="G43">
+        <v>6.9358240024477496E-3</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B44">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C44">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D44">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E44">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F44" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G44">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H44">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B45">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C45">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D45">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E45">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F45" s="1">
+        <v>8.7346677036404701E-4</v>
+      </c>
+      <c r="G45">
+        <v>6.9358240024477496E-3</v>
+      </c>
+      <c r="H45">
+        <v>445.58589874099602</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B46">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C46">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D46">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E46">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F46" s="1">
+        <v>8.7346677036404701E-4</v>
+      </c>
+      <c r="G46">
+        <v>6.9358240024477496E-3</v>
+      </c>
+      <c r="H46">
+        <v>453.23312063998799</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B47">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C47">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D47">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E47">
+        <v>1.3435531643321799E-2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>5.3617953887028099E-4</v>
+      </c>
+      <c r="G47">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H47">
+        <v>512.317409397338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4.0376878128915701</v>
+      </c>
+      <c r="B48">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C48">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D48">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E48">
+        <v>6.3352888103114596E-2</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G48">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B49">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C49">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D49">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E49">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G49">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H49">
+        <v>538.94624827593304</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2.6970619055654099</v>
+      </c>
+      <c r="B50">
+        <v>3.5236804696045301</v>
+      </c>
+      <c r="C50">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D50">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E50">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G50">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H50">
+        <v>366.18216772156399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B51">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C51">
+        <v>2.1355311001063901</v>
+      </c>
+      <c r="D51">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1.03831680301976E-4</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1.5776708763222299E-4</v>
+      </c>
+      <c r="G51">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B52">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C52">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D52">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E52">
+        <v>1.3435531643321799E-2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>5.3617953887028099E-4</v>
+      </c>
+      <c r="G52">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H52">
+        <v>522.02507982748398</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B53">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C53">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D53">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E53">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F53" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G53">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H53">
+        <v>538.94624827593304</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B54">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C54">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D54">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E54">
+        <v>5.5081619122671101E-2</v>
+      </c>
+      <c r="F54" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G54">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B55">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C55">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D55">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E55">
+        <v>2.5329827925644099E-2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G55">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H55">
+        <v>538.94624827593304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B56">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C56">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D56">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E56">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F56" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G56">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H56">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B57">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C57">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D57">
+        <v>6.5854883870776302</v>
+      </c>
+      <c r="E57">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F57" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G57">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2.68673476605507</v>
+      </c>
+      <c r="B58">
+        <v>3.33393969646204</v>
+      </c>
+      <c r="C58">
+        <v>4.7483379530108403</v>
+      </c>
+      <c r="D58">
+        <v>2.3232174857717101</v>
+      </c>
+      <c r="E58">
+        <v>7.9594392867712804E-2</v>
+      </c>
+      <c r="F58" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G58">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B59">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C59">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D59">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E59">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F59" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G59">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H59">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B60">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C60">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D60">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E60">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F60" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G60">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H60">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B61">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C61">
+        <v>3.4311339142875399</v>
+      </c>
+      <c r="D61">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E61">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F61" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G61">
+        <v>2.2614427792349199E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B62">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C62">
+        <v>3.4311339142875399</v>
+      </c>
+      <c r="D62">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E62">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F62" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G62">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H62">
+        <v>376.488542110776</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B63">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C63">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D63">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E63">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F63" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G63">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H63">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B64">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C64">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D64">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E64">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F64" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G64">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H64">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B65">
+        <v>5.6333047435098802</v>
+      </c>
+      <c r="C65">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D65">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E65">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F65" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G65">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B66">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C66">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D66">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E66">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F66" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G66">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H66">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B67">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C67">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D67">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E67">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F67" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G67">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H67">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B68">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C68">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D68">
+        <v>1.5324608412624601</v>
+      </c>
+      <c r="E68">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F68" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G68">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H68">
+        <v>485.50044499686999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B69">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C69">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D69">
+        <v>3.2810981047754399</v>
+      </c>
+      <c r="E69">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F69" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G69">
+        <v>3.01188606191332E-3</v>
+      </c>
+      <c r="H69">
+        <v>530.45523209496002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B70">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C70">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D70">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E70">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F70" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G70">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H70">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B71">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C71">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D71">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E71">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F71" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G71">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H71">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B72">
+        <v>2.0052581720771099</v>
+      </c>
+      <c r="C72">
+        <v>2.7769817684478899</v>
+      </c>
+      <c r="D72">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E72">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F72" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G72">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B73">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C73">
+        <v>6.5992908652451998</v>
+      </c>
+      <c r="D73">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E73">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F73" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G73">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H73">
+        <v>425.304259901607</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B74">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C74">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D74">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E74">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F74" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G74">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H74">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B75">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C75">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D75">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E75">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F75" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G75">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H75">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>3.9874153857952699</v>
+      </c>
+      <c r="B76">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C76">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D76">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E76">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F76" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G76">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H76">
+        <v>390.19653270566499</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B77">
+        <v>5.2481551215459401</v>
+      </c>
+      <c r="C77">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D77">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E77">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F77" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G77">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B78">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C78">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D78">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E78">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F78" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G78">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H78">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B79">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C79">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D79">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E79">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F79" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G79">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H79">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B80">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C80">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D80">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E80">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F80" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G80">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H80">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B81">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C81">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D81">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E81">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F81" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G81">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H81">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B82">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C82">
+        <v>3.12814596586442</v>
+      </c>
+      <c r="D82">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E82">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F82" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G82">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H82">
+        <v>428.07770015489001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B83">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C83">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D83">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E83">
+        <v>4.2129615522282201E-3</v>
+      </c>
+      <c r="F83" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G83">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B84">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C84">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D84">
+        <v>5.8357643078010399</v>
+      </c>
+      <c r="E84">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F84" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G84">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B85">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C85">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D85">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E85">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F85" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G85">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H85">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B86">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C86">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D86">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E86">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F86" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G86">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H86">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B87">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C87">
+        <v>4.0892799627619496</v>
+      </c>
+      <c r="D87">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E87">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F87" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G87">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H87">
+        <v>460.22053226189701</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B88">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C88">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D88">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E88">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F88" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G88">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H88">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B89">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C89">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D89">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E89">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G89">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H89">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B90">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C90">
+        <v>5.1936578966429501</v>
+      </c>
+      <c r="D90">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E90">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F90" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G90">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H90">
+        <v>473.905886833088</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B92">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C92">
+        <v>4.1586188211370203</v>
+      </c>
+      <c r="D92">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E92">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F92" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G92">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H92">
+        <v>421.00730397224902</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B93">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C93">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D93">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E93">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F93" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G93">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H93">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B94">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C94">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D94">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E94">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F94" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G94">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H94">
+        <v>306.50225148772</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B95">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C95">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D95">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E95">
+        <v>2.6102333291748801E-2</v>
+      </c>
+      <c r="F95" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G95">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B96">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C96">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D96">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E96">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F96" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G96">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H96">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B97">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C97">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D97">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E97">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F97" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G97">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H97">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B98">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C98">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D98">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E98">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F98" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G98">
+        <v>6.0261958758608099E-3</v>
+      </c>
+      <c r="H98">
+        <v>471.757528457273</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B99">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C99">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D99">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E99">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F99" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G99">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H99">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B100">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C100">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D100">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E100">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F100" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G100">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H100">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5.0988106698212503</v>
+      </c>
+      <c r="B101">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C101">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D101">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E101">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F101" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G101">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H101">
+        <v>267.20344062837199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B102">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C102">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D102">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E102">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F102" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G102">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H102">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B103">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C103">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D103">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E103">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F103" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G103">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H103">
+        <v>552.15685128966595</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B104">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C104">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D104">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E104">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F104" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G104">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H104">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B105">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C105">
+        <v>5.0061518027585699</v>
+      </c>
+      <c r="D105">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E105">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F105" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G105">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H105">
+        <v>517.52365965185095</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B106">
+        <v>1.1655183374826901</v>
+      </c>
+      <c r="C106">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D106">
+        <v>3.1112957594861701</v>
+      </c>
+      <c r="E106">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F106" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G106">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H106">
+        <v>361.65957176648402</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B107">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C107">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D107">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E107">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F107" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G107">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H107">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B108">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C108">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D108">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E108">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F108" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G108">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H108">
+        <v>576.54274471954295</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B109">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C109">
+        <v>6.4058092979039198</v>
+      </c>
+      <c r="D109">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E109">
+        <v>8.0685187550918205E-2</v>
+      </c>
+      <c r="F109" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G109">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B110">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C110">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D110">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E110">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F110" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G110">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H110">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B111">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C111">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D111">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E111">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F111" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G111">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H111">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>5.2680986922637798</v>
+      </c>
+      <c r="B112">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C112">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D112">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E112">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F112" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G112">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H112">
+        <v>363.45933694383501</v>
+      </c>
+    </row>
+    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B113">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C113">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D113">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E113">
+        <v>4.5772317791518698E-2</v>
+      </c>
+      <c r="F113" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G113">
+        <v>4.49924554788748E-3</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B114">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C114">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D114">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E114">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F114" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G114">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H114">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B115">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C115">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D115">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E115">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F115" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G115">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H115">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>4.7640287857310604</v>
+      </c>
+      <c r="B116">
+        <v>2.9891279977213401</v>
+      </c>
+      <c r="C116">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D116">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E116">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F116" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G116">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B117">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C117">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D117">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E117">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F117" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G117">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H117">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B118">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C118">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D118">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E118">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F118" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G118">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H118">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B119">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C119">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D119">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E119">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F119" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G119">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H119">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="120" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B120">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C120">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D120">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E120">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F120" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G120">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H120">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B121">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C121">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D121">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E121">
+        <v>9.2505144551973298E-2</v>
+      </c>
+      <c r="F121" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G121">
+        <v>3.3536667117185699E-3</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B122">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C122">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D122">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E122">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F122" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G122">
+        <v>2.2614427792349199E-3</v>
+      </c>
+      <c r="H122">
+        <v>577.33830246562502</v>
+      </c>
+    </row>
+    <row r="123" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2.3951030677587601</v>
+      </c>
+      <c r="B123">
+        <v>2.7144312527596002</v>
+      </c>
+      <c r="C123">
+        <v>5.1492553762487798</v>
+      </c>
+      <c r="D123">
+        <v>5.1500786148673097</v>
+      </c>
+      <c r="E123">
+        <v>1.1836134200113599E-2</v>
+      </c>
+      <c r="F123" s="1">
+        <v>3.4381276838257603E-4</v>
+      </c>
+      <c r="G123">
+        <v>2.2614427792349199E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>8</v>
       </c>
-      <c r="B29">
+      <c r="B124">
         <v>461.12158620230099</v>
       </c>
-      <c r="C29">
+      <c r="C124">
         <v>461.12158620230099</v>
       </c>
-      <c r="D29">
+      <c r="D124">
         <v>461.12158620230099</v>
       </c>
-      <c r="E29">
+      <c r="E124">
         <v>461.12158620230099</v>
       </c>
-      <c r="F29">
+      <c r="F124">
         <v>461.12158620230099</v>
       </c>
-      <c r="G29">
+      <c r="G124">
         <v>505.98692982442702</v>
       </c>
-      <c r="H29">
+      <c r="H124">
         <v>505.98692982442702</v>
       </c>
-      <c r="I29">
+      <c r="I124">
         <v>505.98692982442702</v>
+      </c>
+      <c r="J124">
+        <v>505.98692982442702</v>
+      </c>
+      <c r="K124">
+        <v>505.98692982442702</v>
+      </c>
+      <c r="L124">
+        <v>505.98692982442702</v>
+      </c>
+      <c r="M124">
+        <v>505.98692982442702</v>
+      </c>
+      <c r="N124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="O124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="P124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="Q124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="R124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="S124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="T124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="U124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="V124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="W124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="X124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="Y124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="Z124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="AA124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="AB124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="AC124">
+        <v>552.15685128966595</v>
+      </c>
+      <c r="AD124">
+        <v>577.33830246562502</v>
+      </c>
+      <c r="AE124">
+        <v>577.33830246562502</v>
+      </c>
+      <c r="AF124">
+        <v>577.33830246562502</v>
+      </c>
+      <c r="AG124">
+        <v>577.33830246562502</v>
+      </c>
+      <c r="AH124">
+        <v>577.33830246562502</v>
+      </c>
+      <c r="AI124">
+        <v>577.33830246562502</v>
+      </c>
+      <c r="AJ124">
+        <v>577.33830246562502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>